<commit_message>
Add more graphs + excel spreadsheet for the Visual Studio results. Split Readme into libstdc++ and MSVC editions.
</commit_message>
<xml_diff>
--- a/libstdc++.xlsx
+++ b/libstdc++.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="140" windowWidth="22980" windowHeight="8840"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="22980" windowHeight="8835" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="all" sheetId="1" r:id="rId1"/>
+    <sheet name="Sorted" sheetId="1" r:id="rId1"/>
+    <sheet name="Compared" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="88">
   <si>
     <t>Seconds</t>
   </si>
@@ -278,16 +279,13 @@
   </si>
   <si>
     <t>libstdc++-5</t>
-  </si>
-  <si>
-    <t>libstdc++-8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -721,7 +719,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -764,11 +762,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -808,18 +808,34 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -843,18 +859,21 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>all!$D$3</c:f>
+              <c:f>Sorted!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -863,9 +882,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>all!$E$4:$E$83</c:f>
+              <c:f>Sorted!$E$4:$E$83</c:f>
               <c:strCache>
                 <c:ptCount val="80"/>
                 <c:pt idx="0">
@@ -1113,7 +1133,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all!$D$4:$D$83</c:f>
+              <c:f>Sorted!$D$4:$D$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="80"/>
@@ -1361,38 +1381,56 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="226781056"/>
-        <c:axId val="226782592"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="95030272"/>
+        <c:axId val="85870272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="226781056"/>
+        <c:axId val="95030272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="226782592"/>
+        <c:crossAx val="85870272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="226782592"/>
+        <c:axId val="85870272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="226781056"/>
+        <c:crossAx val="95030272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1404,7 +1442,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1428,18 +1476,21 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>all!$D$3</c:f>
+              <c:f>Sorted!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1448,9 +1499,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>all!$H$4:$H$83</c:f>
+              <c:f>Sorted!$H$4:$H$83</c:f>
               <c:strCache>
                 <c:ptCount val="79"/>
                 <c:pt idx="0">
@@ -1695,7 +1747,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all!$G$4:$G$83</c:f>
+              <c:f>Sorted!$G$4:$G$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="80"/>
@@ -1940,38 +1992,56 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="123691776"/>
-        <c:axId val="123694080"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="55324672"/>
+        <c:axId val="50769856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="123691776"/>
+        <c:axId val="55324672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123694080"/>
+        <c:crossAx val="50769856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="123694080"/>
+        <c:axId val="50769856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123691776"/>
+        <c:crossAx val="55324672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1983,7 +2053,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2007,18 +2087,21 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>all!$D$3</c:f>
+              <c:f>Sorted!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2027,9 +2110,10 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>all!$K$4:$K$83</c:f>
+              <c:f>Sorted!$K$4:$K$83</c:f>
               <c:strCache>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
@@ -2265,7 +2349,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>all!$J$4:$J$83</c:f>
+              <c:f>Sorted!$J$4:$J$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="80"/>
@@ -2501,42 +2585,1192 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="123937920"/>
-        <c:axId val="123978496"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="55325184"/>
+        <c:axId val="50771584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="123937920"/>
+        <c:axId val="55325184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123978496"/>
+        <c:crossAx val="50771584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="123978496"/>
+        <c:axId val="50771584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123937920"/>
+        <c:crossAx val="55325184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Mean increase 5 -&gt; 7 is 25.7% (2015-2017)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Compared!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>libstdc++-5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Compared!$J$4:$J$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="80"/>
+                <c:pt idx="0">
+                  <c:v>1.953125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.609375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.953125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.171875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.921875</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.125E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.171875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.6875E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5625E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.25E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.109375</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.46875</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.859375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.6875</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.109375</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.234375</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.8125E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.203125</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.34375</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.140625</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.203125</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.34375</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.328125</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.890625</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.421875</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.765625</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.109375</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.46875</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.609375</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.3125</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.796875</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.78125</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.9375</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.234375</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.265625</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.171875</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.53125</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.28125</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.21875</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.4375</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.953125</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.71875</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.984375</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>7.203125</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.296875</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>7.21875</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.1875</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.65625</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.828125</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.90625</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.578125</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.953125</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.21875</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.984375</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.09375</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.09375</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5.046875</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.3125</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.28125</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.140625</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.5625</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.609375</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.515625</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.96875</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.53125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Compared!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>libstdc++-6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Compared!$G$4:$G$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="80"/>
+                <c:pt idx="0">
+                  <c:v>1.984375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.984375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.171875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.765625</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.171875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.109375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.234375</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.703125</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.765625</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.375</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.265625</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.109375</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.109375</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.234375</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.265625</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.1875</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.21875</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.328125</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.15625</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.671875</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.484375</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.078125</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.46875</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.015625</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.109375</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.78125</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.609375</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.328125</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.765625</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.734375</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.921875</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.546875</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.28125</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.640625</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.40625</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.40625</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.171875</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.484375</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.90625</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.625</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.015625</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.15625</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.328125</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>7.828125</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.28125</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.6875</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.453125</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.90625</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.625</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2.859375</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.171875</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2.875</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.046875</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.09375</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5.109375</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.328125</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.3125</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.640625</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.71875</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.640625</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.671875</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.5625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Compared!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>libstdc++-7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Compared!$E$4:$E$83</c:f>
+              <c:strCache>
+                <c:ptCount val="80"/>
+                <c:pt idx="0">
+                  <c:v>algorithm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>any</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>array</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>atomic</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>bitset</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>cassert</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cctype</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cerrno</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>cfenv</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>cfloat</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>chrono</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>cinttypes</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>climits</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>clocale</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>cmath</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>codecvt</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>complex</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>condition_variable</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>csetjmp</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>csignal</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>cstdarg</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>cstddef</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>cstdint</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>cstdio</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>cstdlib</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>cstring</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>ctime</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>cuchar</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>cwchar</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>cwctype</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>deque</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>exception</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>experimental/filesystem</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>experimental/memory_resource</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>forward_list</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>fstream</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>functional</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>future</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>initializer_list</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>iomanip</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>ios</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>iosfwd</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>iostream</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>istream</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>iterator</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>limits</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>list</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>locale</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>map</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>memory</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>mutex</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>new</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>numeric</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>optional</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>ostream</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>queue</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>random</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>ratio</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>regex</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>scoped_allocator</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>set</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>shared_mutex</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>sstream</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>stack</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>stdexcept</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>streambuf</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>string</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>string_view</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>system_error</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>thread</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>tuple</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>type_traits</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>typeindex</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>typeinfo</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>unordered_map</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>unordered_set</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>utility</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>valarray</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>variant</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>vector</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Compared!$D$4:$D$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="80"/>
+                <c:pt idx="0">
+                  <c:v>2.34375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.015625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.609375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.453125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.171875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.71875</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.109375</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.109375</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.59375</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.484375</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.109375</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.28125</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.109375</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.234375</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.109375</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.109375</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.234375</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.140625</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.171875</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.171875</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.984375</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.625</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.15625</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.390625</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.8125</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.671875</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.234375</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.765625</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.109375</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.515625</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.328125</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.484375</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.3125</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.546875</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.21875</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.078125</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.734375</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.21875</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.78125</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.671875</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.65625</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.71875</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.328125</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.59375</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.515625</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.34375</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>8.875</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.109375</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.515625</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.40625</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.546875</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.796875</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.484375</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.59375</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.640625</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.046875</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.328125</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.140625</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.71875</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.78125</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.96875</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.5625</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.859375</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2.4375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="50793984"/>
+        <c:axId val="50773312"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50793984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50773312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50773312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50793984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2637,6 +3871,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19048</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>433576</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2712,6 +3981,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2746,6 +4016,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2921,19 +4192,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="Q4" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
-        <v>88</v>
-      </c>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>82</v>
       </c>
@@ -2944,15 +4212,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="e">
-        <f>AVERAGE(A4:A100)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B2" t="e">
-        <f>MEDIAN(A4:A100)</f>
-        <v>#NUM!</v>
-      </c>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
       <c r="D2">
         <f>AVERAGE(D4:D100)</f>
         <v>2.5314453124999998</v>
@@ -2978,7 +4240,7 @@
         <v>1.5546875</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>0</v>
       </c>
@@ -2998,7 +4260,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
       <c r="D4">
         <v>9.375E-2</v>
       </c>
@@ -3018,7 +4282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>9.375E-2</v>
       </c>
@@ -3038,7 +4302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>9.375E-2</v>
       </c>
@@ -3058,7 +4322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>9.375E-2</v>
       </c>
@@ -3078,7 +4342,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>0.109375</v>
       </c>
@@ -3098,7 +4362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>0.109375</v>
       </c>
@@ -3118,7 +4382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D10">
         <v>0.109375</v>
       </c>
@@ -3138,7 +4402,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>0.109375</v>
       </c>
@@ -3158,7 +4422,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>0.109375</v>
       </c>
@@ -3178,7 +4442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>0.109375</v>
       </c>
@@ -3198,7 +4462,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>0.125</v>
       </c>
@@ -3218,7 +4482,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>0.125</v>
       </c>
@@ -3238,7 +4502,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>0.140625</v>
       </c>
@@ -3258,7 +4522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="4:11">
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17">
         <v>0.140625</v>
       </c>
@@ -3278,7 +4542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="4:11">
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18">
         <v>0.15625</v>
       </c>
@@ -3298,7 +4562,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="4:11">
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>0.15625</v>
       </c>
@@ -3318,7 +4582,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="4:11">
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>0.171875</v>
       </c>
@@ -3338,7 +4602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="4:11">
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>0.171875</v>
       </c>
@@ -3358,7 +4622,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="4:11">
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D22">
         <v>0.171875</v>
       </c>
@@ -3378,7 +4642,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="4:11">
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D23">
         <v>0.21875</v>
       </c>
@@ -3398,7 +4662,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="4:11">
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D24">
         <v>0.234375</v>
       </c>
@@ -3418,7 +4682,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="4:11">
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D25">
         <v>0.234375</v>
       </c>
@@ -3438,7 +4702,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="4:11">
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D26">
         <v>0.25</v>
       </c>
@@ -3458,7 +4722,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="4:11">
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D27">
         <v>0.25</v>
       </c>
@@ -3478,7 +4742,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="4:11">
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D28">
         <v>0.328125</v>
       </c>
@@ -3498,7 +4762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="4:11">
+    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D29">
         <v>0.328125</v>
       </c>
@@ -3518,7 +4782,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="4:11">
+    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D30">
         <v>0.34375</v>
       </c>
@@ -3538,7 +4802,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="4:11">
+    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D31">
         <v>0.4375</v>
       </c>
@@ -3558,7 +4822,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="4:11">
+    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D32">
         <v>0.625</v>
       </c>
@@ -3578,7 +4842,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="4:11">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33">
         <v>0.65625</v>
       </c>
@@ -3598,7 +4862,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="4:11">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>0.671875</v>
       </c>
@@ -3618,7 +4882,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="4:11">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35">
         <v>0.71875</v>
       </c>
@@ -3638,7 +4902,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="4:11">
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36">
         <v>0.96875</v>
       </c>
@@ -3658,7 +4922,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="4:11">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37">
         <v>1.015625</v>
       </c>
@@ -3678,7 +4942,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="4:11">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38">
         <v>1.59375</v>
       </c>
@@ -3698,7 +4962,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="4:11">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>1.59375</v>
       </c>
@@ -3718,7 +4982,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="4:11">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40">
         <v>1.75</v>
       </c>
@@ -3738,7 +5002,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="4:11">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41">
         <v>1.8125</v>
       </c>
@@ -3758,7 +5022,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="4:11">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42">
         <v>1.859375</v>
       </c>
@@ -3778,7 +5042,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="4:11">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43">
         <v>1.984375</v>
       </c>
@@ -3798,7 +5062,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="4:11">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44">
         <v>2.25</v>
       </c>
@@ -3818,7 +5082,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="4:11">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45">
         <v>2.34375</v>
       </c>
@@ -3838,7 +5102,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="4:11">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46">
         <v>2.4375</v>
       </c>
@@ -3858,7 +5122,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="4:11">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47">
         <v>2.59375</v>
       </c>
@@ -3878,7 +5142,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="4:11">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48">
         <v>3.453125</v>
       </c>
@@ -3898,7 +5162,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="4:11">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49">
         <v>3.484375</v>
       </c>
@@ -3918,7 +5182,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="4:11">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50">
         <v>3.484375</v>
       </c>
@@ -3938,7 +5202,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="4:11">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51">
         <v>3.5</v>
       </c>
@@ -3958,7 +5222,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="4:11">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52">
         <v>3.5625</v>
       </c>
@@ -3978,7 +5242,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="4:11">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53">
         <v>3.609375</v>
       </c>
@@ -3998,7 +5262,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="4:11">
+    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D54">
         <v>3.640625</v>
       </c>
@@ -4018,7 +5282,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="4:11">
+    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D55">
         <v>3.71875</v>
       </c>
@@ -4038,7 +5302,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="4:11">
+    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D56">
         <v>3.796875</v>
       </c>
@@ -4058,7 +5322,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="4:11">
+    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D57">
         <v>4.046875</v>
       </c>
@@ -4078,7 +5342,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="4:11">
+    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D58">
         <v>4.109375</v>
       </c>
@@ -4098,7 +5362,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="4:11">
+    <row r="59" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D59">
         <v>4.3125</v>
       </c>
@@ -4118,7 +5382,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="4:11">
+    <row r="60" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D60">
         <v>4.328125</v>
       </c>
@@ -4138,7 +5402,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="4:11">
+    <row r="61" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D61">
         <v>4.484375</v>
       </c>
@@ -4158,7 +5422,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="4:11">
+    <row r="62" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D62">
         <v>4.515625</v>
       </c>
@@ -4178,7 +5442,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="4:11">
+    <row r="63" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D63">
         <v>4.515625</v>
       </c>
@@ -4198,7 +5462,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="4:11">
+    <row r="64" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D64">
         <v>4.546875</v>
       </c>
@@ -4218,7 +5482,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="4:11">
+    <row r="65" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D65">
         <v>4.546875</v>
       </c>
@@ -4238,7 +5502,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="4:11">
+    <row r="66" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D66">
         <v>4.671875</v>
       </c>
@@ -4258,7 +5522,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="4:11">
+    <row r="67" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D67">
         <v>4.71875</v>
       </c>
@@ -4278,7 +5542,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="68" spans="4:11">
+    <row r="68" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D68">
         <v>4.734375</v>
       </c>
@@ -4298,7 +5562,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="4:11">
+    <row r="69" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D69">
         <v>4.78125</v>
       </c>
@@ -4318,7 +5582,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="4:11">
+    <row r="70" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D70">
         <v>4.78125</v>
       </c>
@@ -4338,7 +5602,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="4:11">
+    <row r="71" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D71">
         <v>5.078125</v>
       </c>
@@ -4358,7 +5622,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="4:11">
+    <row r="72" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D72">
         <v>5.109375</v>
       </c>
@@ -4378,7 +5642,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="4:11">
+    <row r="73" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D73">
         <v>5.21875</v>
       </c>
@@ -4398,7 +5662,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="74" spans="4:11">
+    <row r="74" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D74">
         <v>5.28125</v>
       </c>
@@ -4418,7 +5682,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="4:11">
+    <row r="75" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D75">
         <v>5.390625</v>
       </c>
@@ -4438,7 +5702,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="4:11">
+    <row r="76" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D76">
         <v>5.40625</v>
       </c>
@@ -4458,7 +5722,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="4:11">
+    <row r="77" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D77">
         <v>5.5</v>
       </c>
@@ -4478,7 +5742,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="4:11">
+    <row r="78" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D78">
         <v>5.515625</v>
       </c>
@@ -4498,7 +5762,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="4:11">
+    <row r="79" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D79">
         <v>5.75</v>
       </c>
@@ -4518,7 +5782,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="4:11">
+    <row r="80" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D80">
         <v>6.234375</v>
       </c>
@@ -4532,7 +5796,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="4:8">
+    <row r="81" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D81">
         <v>6.765625</v>
       </c>
@@ -4546,7 +5810,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="4:8">
+    <row r="82" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D82">
         <v>7.15625</v>
       </c>
@@ -4560,7 +5824,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="4:8">
+    <row r="83" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D83">
         <v>8.875</v>
       </c>
@@ -4572,4 +5836,1658 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>(D2-J2)/J2</f>
+        <v>0.25667993468054684</v>
+      </c>
+      <c r="B2">
+        <f>(E2-K2)/K2</f>
+        <v>0.36180904522613067</v>
+      </c>
+      <c r="D2">
+        <f>AVERAGE(D4:D100)</f>
+        <v>2.5314453124999998</v>
+      </c>
+      <c r="E2">
+        <f>MEDIAN(D4:D100)</f>
+        <v>2.1171875</v>
+      </c>
+      <c r="G2">
+        <f>AVERAGE(G4:G100)</f>
+        <v>2.0528085443037973</v>
+      </c>
+      <c r="H2">
+        <f>MEDIAN(G4:G100)</f>
+        <v>1.625</v>
+      </c>
+      <c r="J2">
+        <f>AVERAGE(J4:J100)</f>
+        <v>2.0143914473684212</v>
+      </c>
+      <c r="K2">
+        <f>MEDIAN(J4:J100)</f>
+        <v>1.5546875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>2.34375</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4">
+        <v>1.984375</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4">
+        <v>1.953125</v>
+      </c>
+      <c r="K4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1.015625</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5">
+        <v>0.78125</v>
+      </c>
+      <c r="H5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5">
+        <v>0.609375</v>
+      </c>
+      <c r="K5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>3.609375</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6">
+        <v>2.984375</v>
+      </c>
+      <c r="H6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6">
+        <v>2.953125</v>
+      </c>
+      <c r="K6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0.4375</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7">
+        <v>0.171875</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7">
+        <v>0.171875</v>
+      </c>
+      <c r="K7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>3.453125</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8">
+        <v>2.765625</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8">
+        <v>2.921875</v>
+      </c>
+      <c r="K8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>9.375E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>9.375E-2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>0.171875</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10">
+        <v>0.171875</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10">
+        <v>0.171875</v>
+      </c>
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>9.375E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <v>9.375E-2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11">
+        <v>4.6875E-2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>0.125</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>0.109375</v>
+      </c>
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <v>0.125</v>
+      </c>
+      <c r="K12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>9.375E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>9.375E-2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="K13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>0.71875</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14">
+        <v>0.625</v>
+      </c>
+      <c r="H14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14">
+        <v>0.625</v>
+      </c>
+      <c r="K14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>0.125</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>0.125</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15">
+        <v>0.125</v>
+      </c>
+      <c r="K15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>0.109375</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <v>9.375E-2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16">
+        <v>6.25E-2</v>
+      </c>
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0.109375</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>0.125</v>
+      </c>
+      <c r="H17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17">
+        <v>0.109375</v>
+      </c>
+      <c r="K17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>1.59375</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18">
+        <v>0.234375</v>
+      </c>
+      <c r="H18" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18">
+        <v>0.46875</v>
+      </c>
+      <c r="K18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>3.484375</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19">
+        <v>2.703125</v>
+      </c>
+      <c r="H19" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19">
+        <v>2.859375</v>
+      </c>
+      <c r="K19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>5.109375</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20">
+        <v>3.765625</v>
+      </c>
+      <c r="H20" t="s">
+        <v>71</v>
+      </c>
+      <c r="J20">
+        <v>4.25</v>
+      </c>
+      <c r="K20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>5.28125</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21">
+        <v>4.375</v>
+      </c>
+      <c r="H21" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21">
+        <v>4.6875</v>
+      </c>
+      <c r="K21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>0.109375</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22">
+        <v>0.125</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22">
+        <v>0.109375</v>
+      </c>
+      <c r="K22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>0.234375</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23">
+        <v>0.265625</v>
+      </c>
+      <c r="H23" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23">
+        <v>0.234375</v>
+      </c>
+      <c r="K23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>9.375E-2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>0.109375</v>
+      </c>
+      <c r="H24" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24">
+        <v>9.375E-2</v>
+      </c>
+      <c r="K24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>0.109375</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <v>0.109375</v>
+      </c>
+      <c r="H25" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <v>7.8125E-2</v>
+      </c>
+      <c r="K25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>0.109375</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>0.125</v>
+      </c>
+      <c r="H26" t="s">
+        <v>5</v>
+      </c>
+      <c r="J26">
+        <v>9.375E-2</v>
+      </c>
+      <c r="K26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>0.234375</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27">
+        <v>0.234375</v>
+      </c>
+      <c r="H27" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27">
+        <v>0.203125</v>
+      </c>
+      <c r="K27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>0.140625</v>
+      </c>
+      <c r="E28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28">
+        <v>9.375E-2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28">
+        <v>0.34375</v>
+      </c>
+      <c r="K28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>0.15625</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29">
+        <v>0.125</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29">
+        <v>0.125</v>
+      </c>
+      <c r="K29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>0.171875</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30">
+        <v>0.15625</v>
+      </c>
+      <c r="H30" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30">
+        <v>0.140625</v>
+      </c>
+      <c r="K30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>0.25</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31">
+        <v>0.265625</v>
+      </c>
+      <c r="H31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>0.171875</v>
+      </c>
+      <c r="E32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32">
+        <v>0.1875</v>
+      </c>
+      <c r="H32" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32">
+        <v>0.15625</v>
+      </c>
+      <c r="K32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>0.25</v>
+      </c>
+      <c r="E33" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33">
+        <v>0.21875</v>
+      </c>
+      <c r="H33" t="s">
+        <v>22</v>
+      </c>
+      <c r="J33">
+        <v>0.203125</v>
+      </c>
+      <c r="K33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>1.984375</v>
+      </c>
+      <c r="E34" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34">
+        <v>1.328125</v>
+      </c>
+      <c r="H34" t="s">
+        <v>41</v>
+      </c>
+      <c r="J34">
+        <v>1.34375</v>
+      </c>
+      <c r="K34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>0.625</v>
+      </c>
+      <c r="E35" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35">
+        <v>9.375E-2</v>
+      </c>
+      <c r="H35" t="s">
+        <v>30</v>
+      </c>
+      <c r="J35">
+        <v>9.375E-2</v>
+      </c>
+      <c r="K35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>7.15625</v>
+      </c>
+      <c r="E36" t="s">
+        <v>80</v>
+      </c>
+      <c r="G36">
+        <v>6.15625</v>
+      </c>
+      <c r="H36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>5.390625</v>
+      </c>
+      <c r="E37" t="s">
+        <v>73</v>
+      </c>
+      <c r="G37">
+        <v>4.671875</v>
+      </c>
+      <c r="H37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>1.8125</v>
+      </c>
+      <c r="E38" t="s">
+        <v>38</v>
+      </c>
+      <c r="G38">
+        <v>1.484375</v>
+      </c>
+      <c r="H38" t="s">
+        <v>38</v>
+      </c>
+      <c r="J38">
+        <v>1.328125</v>
+      </c>
+      <c r="K38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>4.671875</v>
+      </c>
+      <c r="E39" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39">
+        <v>4.078125</v>
+      </c>
+      <c r="H39" t="s">
+        <v>65</v>
+      </c>
+      <c r="J39">
+        <v>3.890625</v>
+      </c>
+      <c r="K39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>6.234375</v>
+      </c>
+      <c r="E40" t="s">
+        <v>78</v>
+      </c>
+      <c r="G40">
+        <v>3.46875</v>
+      </c>
+      <c r="H40" t="s">
+        <v>78</v>
+      </c>
+      <c r="J40">
+        <v>3.421875</v>
+      </c>
+      <c r="K40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>6.765625</v>
+      </c>
+      <c r="E41" t="s">
+        <v>79</v>
+      </c>
+      <c r="G41">
+        <v>6.015625</v>
+      </c>
+      <c r="H41" t="s">
+        <v>79</v>
+      </c>
+      <c r="J41">
+        <v>5.765625</v>
+      </c>
+      <c r="K41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>0.109375</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42">
+        <v>0.109375</v>
+      </c>
+      <c r="H42" t="s">
+        <v>11</v>
+      </c>
+      <c r="J42">
+        <v>0.109375</v>
+      </c>
+      <c r="K42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>5.5</v>
+      </c>
+      <c r="E43" t="s">
+        <v>76</v>
+      </c>
+      <c r="G43">
+        <v>4.78125</v>
+      </c>
+      <c r="H43" t="s">
+        <v>76</v>
+      </c>
+      <c r="J43">
+        <v>4.46875</v>
+      </c>
+      <c r="K43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>4.515625</v>
+      </c>
+      <c r="E44" t="s">
+        <v>56</v>
+      </c>
+      <c r="G44">
+        <v>3.609375</v>
+      </c>
+      <c r="H44" t="s">
+        <v>56</v>
+      </c>
+      <c r="J44">
+        <v>3.609375</v>
+      </c>
+      <c r="K44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>0.328125</v>
+      </c>
+      <c r="E45" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45">
+        <v>0.328125</v>
+      </c>
+      <c r="H45" t="s">
+        <v>27</v>
+      </c>
+      <c r="J45">
+        <v>0.3125</v>
+      </c>
+      <c r="K45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>4.484375</v>
+      </c>
+      <c r="E46" t="s">
+        <v>60</v>
+      </c>
+      <c r="G46">
+        <v>3.765625</v>
+      </c>
+      <c r="H46" t="s">
+        <v>60</v>
+      </c>
+      <c r="J46">
+        <v>3.796875</v>
+      </c>
+      <c r="K46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>4.3125</v>
+      </c>
+      <c r="E47" t="s">
+        <v>59</v>
+      </c>
+      <c r="G47">
+        <v>3.734375</v>
+      </c>
+      <c r="H47" t="s">
+        <v>59</v>
+      </c>
+      <c r="J47">
+        <v>3.78125</v>
+      </c>
+      <c r="K47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>4.546875</v>
+      </c>
+      <c r="E48" t="s">
+        <v>62</v>
+      </c>
+      <c r="G48">
+        <v>3.921875</v>
+      </c>
+      <c r="H48" t="s">
+        <v>62</v>
+      </c>
+      <c r="J48">
+        <v>3.9375</v>
+      </c>
+      <c r="K48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>0.21875</v>
+      </c>
+      <c r="E49" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49">
+        <v>0.25</v>
+      </c>
+      <c r="H49" t="s">
+        <v>23</v>
+      </c>
+      <c r="J49">
+        <v>0.234375</v>
+      </c>
+      <c r="K49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>1.75</v>
+      </c>
+      <c r="E50" t="s">
+        <v>39</v>
+      </c>
+      <c r="G50">
+        <v>1.546875</v>
+      </c>
+      <c r="H50" t="s">
+        <v>39</v>
+      </c>
+      <c r="J50">
+        <v>1.265625</v>
+      </c>
+      <c r="K50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>5.078125</v>
+      </c>
+      <c r="E51" t="s">
+        <v>69</v>
+      </c>
+      <c r="G51">
+        <v>4.28125</v>
+      </c>
+      <c r="H51" t="s">
+        <v>69</v>
+      </c>
+      <c r="J51">
+        <v>4.171875</v>
+      </c>
+      <c r="K51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>4.734375</v>
+      </c>
+      <c r="E52" t="s">
+        <v>66</v>
+      </c>
+      <c r="G52">
+        <v>3.640625</v>
+      </c>
+      <c r="H52" t="s">
+        <v>66</v>
+      </c>
+      <c r="J52">
+        <v>3.53125</v>
+      </c>
+      <c r="K52" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>5.21875</v>
+      </c>
+      <c r="E53" t="s">
+        <v>70</v>
+      </c>
+      <c r="G53">
+        <v>4.40625</v>
+      </c>
+      <c r="H53" t="s">
+        <v>70</v>
+      </c>
+      <c r="J53">
+        <v>4.28125</v>
+      </c>
+      <c r="K53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>4.78125</v>
+      </c>
+      <c r="E54" t="s">
+        <v>64</v>
+      </c>
+      <c r="G54">
+        <v>4.40625</v>
+      </c>
+      <c r="H54" t="s">
+        <v>64</v>
+      </c>
+      <c r="J54">
+        <v>4.21875</v>
+      </c>
+      <c r="K54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>0.671875</v>
+      </c>
+      <c r="E55" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55">
+        <v>0.171875</v>
+      </c>
+      <c r="H55" t="s">
+        <v>31</v>
+      </c>
+      <c r="J55">
+        <v>0.15625</v>
+      </c>
+      <c r="K55" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>0.65625</v>
+      </c>
+      <c r="E56" t="s">
+        <v>32</v>
+      </c>
+      <c r="G56">
+        <v>0.484375</v>
+      </c>
+      <c r="H56" t="s">
+        <v>32</v>
+      </c>
+      <c r="J56">
+        <v>0.4375</v>
+      </c>
+      <c r="K56" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>3.71875</v>
+      </c>
+      <c r="E57" t="s">
+        <v>53</v>
+      </c>
+      <c r="G57">
+        <v>2.90625</v>
+      </c>
+      <c r="H57" t="s">
+        <v>85</v>
+      </c>
+      <c r="J57">
+        <v>2.953125</v>
+      </c>
+      <c r="K57" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>4.328125</v>
+      </c>
+      <c r="E58" t="s">
+        <v>58</v>
+      </c>
+      <c r="G58">
+        <v>3.625</v>
+      </c>
+      <c r="H58" t="s">
+        <v>58</v>
+      </c>
+      <c r="J58">
+        <v>3.71875</v>
+      </c>
+      <c r="K58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>2.59375</v>
+      </c>
+      <c r="E59" t="s">
+        <v>45</v>
+      </c>
+      <c r="G59">
+        <v>2.015625</v>
+      </c>
+      <c r="H59" t="s">
+        <v>45</v>
+      </c>
+      <c r="J59">
+        <v>1.984375</v>
+      </c>
+      <c r="K59" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>5.515625</v>
+      </c>
+      <c r="E60" t="s">
+        <v>75</v>
+      </c>
+      <c r="G60">
+        <v>4.15625</v>
+      </c>
+      <c r="H60" t="s">
+        <v>75</v>
+      </c>
+      <c r="J60">
+        <v>7.203125</v>
+      </c>
+      <c r="K60" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <v>0.34375</v>
+      </c>
+      <c r="E61" t="s">
+        <v>28</v>
+      </c>
+      <c r="G61">
+        <v>0.328125</v>
+      </c>
+      <c r="H61" t="s">
+        <v>28</v>
+      </c>
+      <c r="J61">
+        <v>0.296875</v>
+      </c>
+      <c r="K61" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <v>8.875</v>
+      </c>
+      <c r="E62" t="s">
+        <v>81</v>
+      </c>
+      <c r="G62">
+        <v>7.828125</v>
+      </c>
+      <c r="H62" t="s">
+        <v>81</v>
+      </c>
+      <c r="J62">
+        <v>7.21875</v>
+      </c>
+      <c r="K62" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <v>4.109375</v>
+      </c>
+      <c r="E63" t="s">
+        <v>57</v>
+      </c>
+      <c r="G63">
+        <v>3.28125</v>
+      </c>
+      <c r="H63" t="s">
+        <v>57</v>
+      </c>
+      <c r="J63">
+        <v>3.1875</v>
+      </c>
+      <c r="K63" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <v>4.515625</v>
+      </c>
+      <c r="E64" t="s">
+        <v>63</v>
+      </c>
+      <c r="G64">
+        <v>1.6875</v>
+      </c>
+      <c r="H64" t="s">
+        <v>63</v>
+      </c>
+      <c r="J64">
+        <v>1.65625</v>
+      </c>
+      <c r="K64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <v>5.40625</v>
+      </c>
+      <c r="E65" t="s">
+        <v>74</v>
+      </c>
+      <c r="G65">
+        <v>4.453125</v>
+      </c>
+      <c r="H65" t="s">
+        <v>74</v>
+      </c>
+      <c r="J65">
+        <v>4.828125</v>
+      </c>
+      <c r="K65" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <v>4.546875</v>
+      </c>
+      <c r="E66" t="s">
+        <v>61</v>
+      </c>
+      <c r="G66">
+        <v>3.90625</v>
+      </c>
+      <c r="H66" t="s">
+        <v>61</v>
+      </c>
+      <c r="J66">
+        <v>3.90625</v>
+      </c>
+      <c r="K66" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <v>2.25</v>
+      </c>
+      <c r="E67" t="s">
+        <v>43</v>
+      </c>
+      <c r="G67">
+        <v>1.625</v>
+      </c>
+      <c r="H67" t="s">
+        <v>43</v>
+      </c>
+      <c r="J67">
+        <v>1.578125</v>
+      </c>
+      <c r="K67" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="68" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <v>3.5</v>
+      </c>
+      <c r="E68" t="s">
+        <v>47</v>
+      </c>
+      <c r="G68">
+        <v>2.859375</v>
+      </c>
+      <c r="H68" t="s">
+        <v>47</v>
+      </c>
+      <c r="J68">
+        <v>2.953125</v>
+      </c>
+      <c r="K68" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <v>3.796875</v>
+      </c>
+      <c r="E69" t="s">
+        <v>54</v>
+      </c>
+      <c r="G69">
+        <v>3.171875</v>
+      </c>
+      <c r="H69" t="s">
+        <v>54</v>
+      </c>
+      <c r="J69">
+        <v>3.21875</v>
+      </c>
+      <c r="K69" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <v>3.484375</v>
+      </c>
+      <c r="E70" t="s">
+        <v>49</v>
+      </c>
+      <c r="G70">
+        <v>2.875</v>
+      </c>
+      <c r="H70" t="s">
+        <v>49</v>
+      </c>
+      <c r="J70">
+        <v>2.984375</v>
+      </c>
+      <c r="K70" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="71" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <v>1.59375</v>
+      </c>
+      <c r="E71" t="s">
+        <v>36</v>
+      </c>
+      <c r="G71">
+        <v>3.046875</v>
+      </c>
+      <c r="H71" t="s">
+        <v>84</v>
+      </c>
+      <c r="J71">
+        <v>3.09375</v>
+      </c>
+      <c r="K71" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <v>3.640625</v>
+      </c>
+      <c r="E72" t="s">
+        <v>52</v>
+      </c>
+      <c r="G72">
+        <v>3.09375</v>
+      </c>
+      <c r="H72" t="s">
+        <v>52</v>
+      </c>
+      <c r="J72">
+        <v>3.09375</v>
+      </c>
+      <c r="K72" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="73" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <v>5.75</v>
+      </c>
+      <c r="E73" t="s">
+        <v>77</v>
+      </c>
+      <c r="G73">
+        <v>5.109375</v>
+      </c>
+      <c r="H73" t="s">
+        <v>77</v>
+      </c>
+      <c r="J73">
+        <v>5.046875</v>
+      </c>
+      <c r="K73" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="74" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>4.046875</v>
+      </c>
+      <c r="E74" t="s">
+        <v>55</v>
+      </c>
+      <c r="G74">
+        <v>3.328125</v>
+      </c>
+      <c r="H74" t="s">
+        <v>55</v>
+      </c>
+      <c r="J74">
+        <v>3.3125</v>
+      </c>
+      <c r="K74" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>0.328125</v>
+      </c>
+      <c r="E75" t="s">
+        <v>26</v>
+      </c>
+      <c r="G75">
+        <v>0.3125</v>
+      </c>
+      <c r="H75" t="s">
+        <v>26</v>
+      </c>
+      <c r="J75">
+        <v>0.28125</v>
+      </c>
+      <c r="K75" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>0.15625</v>
+      </c>
+      <c r="E76" t="s">
+        <v>16</v>
+      </c>
+      <c r="G76">
+        <v>0.15625</v>
+      </c>
+      <c r="H76" t="s">
+        <v>16</v>
+      </c>
+      <c r="J76">
+        <v>0.140625</v>
+      </c>
+      <c r="K76" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>0.140625</v>
+      </c>
+      <c r="E77" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77">
+        <v>0.125</v>
+      </c>
+      <c r="H77" t="s">
+        <v>12</v>
+      </c>
+      <c r="J77">
+        <v>0.125</v>
+      </c>
+      <c r="K77" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <v>4.71875</v>
+      </c>
+      <c r="E78" t="s">
+        <v>67</v>
+      </c>
+      <c r="G78">
+        <v>3.640625</v>
+      </c>
+      <c r="H78" t="s">
+        <v>67</v>
+      </c>
+      <c r="J78">
+        <v>3.5625</v>
+      </c>
+      <c r="K78" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <v>4.78125</v>
+      </c>
+      <c r="E79" t="s">
+        <v>68</v>
+      </c>
+      <c r="G79">
+        <v>3.71875</v>
+      </c>
+      <c r="H79" t="s">
+        <v>68</v>
+      </c>
+      <c r="J79">
+        <v>3.609375</v>
+      </c>
+      <c r="K79" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <v>0.96875</v>
+      </c>
+      <c r="E80" t="s">
+        <v>35</v>
+      </c>
+      <c r="G80">
+        <v>0.640625</v>
+      </c>
+      <c r="H80" t="s">
+        <v>35</v>
+      </c>
+      <c r="J80">
+        <v>0.515625</v>
+      </c>
+      <c r="K80" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <v>3.5625</v>
+      </c>
+      <c r="E81" t="s">
+        <v>46</v>
+      </c>
+      <c r="G81">
+        <v>2.671875</v>
+      </c>
+      <c r="H81" t="s">
+        <v>46</v>
+      </c>
+      <c r="J81">
+        <v>2.96875</v>
+      </c>
+      <c r="K81" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="82" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <v>1.859375</v>
+      </c>
+      <c r="E82" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="83" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <v>2.4375</v>
+      </c>
+      <c r="E83" t="s">
+        <v>42</v>
+      </c>
+      <c r="G83">
+        <v>1.5625</v>
+      </c>
+      <c r="H83" t="s">
+        <v>42</v>
+      </c>
+      <c r="J83">
+        <v>1.53125</v>
+      </c>
+      <c r="K83" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="J4:K79">
+    <sortCondition ref="K4:K79"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>